<commit_message>
ajustando o layout pra receber valor e retornar na forma de valor
</commit_message>
<xml_diff>
--- a/E670RATteste.xlsx
+++ b/E670RATteste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larissa.barcelos\Desktop\Laryssa\Demandas\conversao excel-txt python para erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FF7400-472B-4E98-9111-1EF5136F52C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18AE86D-7165-4385-BEA1-6B938881530E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{D647A2BC-56F8-4232-827C-D44FE2DF9BBE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -33,29 +33,46 @@
     <t>CODIGO BEM</t>
   </si>
   <si>
-    <t>DATA LOCALIZACAO</t>
-  </si>
-  <si>
-    <t>SEQUENCIA</t>
-  </si>
-  <si>
-    <t>CODIGO LOCAL REAL</t>
-  </si>
-  <si>
     <t>9999999999-000</t>
+  </si>
+  <si>
+    <t>DATA MOVIMENTACAO</t>
+  </si>
+  <si>
+    <t>SEQUENCIA MOV</t>
+  </si>
+  <si>
+    <t>SEQUENCIA RATEIO</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>COD C CUSTO</t>
+  </si>
+  <si>
+    <t>PERC RATEIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,9 +95,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,21 +416,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68C344C-22D3-43F8-9AE2-56C3DE0CD553}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,21 +439,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>45900</v>
@@ -440,7 +471,16 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>301</v>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2">
+        <v>100</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2000.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mais um campo adicionado por ser obrigatório
</commit_message>
<xml_diff>
--- a/E670RATteste.xlsx
+++ b/E670RATteste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larissa.barcelos\Desktop\Laryssa\Demandas\conversao excel-txt python para erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18AE86D-7165-4385-BEA1-6B938881530E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623F9D8-A930-4354-8895-123C2A1281AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{D647A2BC-56F8-4232-827C-D44FE2DF9BBE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -52,16 +52,20 @@
   </si>
   <si>
     <t>PERC RATEIO</t>
+  </si>
+  <si>
+    <t>COD ESPECIE BEM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="#,##0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +77,20 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,13 +113,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68C344C-22D3-43F8-9AE2-56C3DE0CD553}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,9 +451,10 @@
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,32 +479,114 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>45900</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="3">
+        <v>45894</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1">
+        <v>100</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2000.5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45894</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
         <v>65</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="6">
         <v>100</v>
       </c>
-      <c r="H2" s="3">
-        <v>2000.5</v>
-      </c>
+      <c r="H3" s="4">
+        <v>1500.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>